<commit_message>
Updated Scrum Master Log and added new Sprint backlog.
</commit_message>
<xml_diff>
--- a/project/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/project/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\ES\Projects\SE2122-57672-58175-57957-58210-57911\project\Phase 1\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao4\IdeaProjects\SE2122-57672-58175-57957-58210-57911\project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC42FD-4BCE-42D8-8916-173B822797D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A7FF38-178F-41B3-A648-D0329BBE968B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Detect code smells.</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>This backlog doesn't have tasks separated by each member as we all had something to do from each one of the tasks or did the remaining ones together</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Not yet started</t>
   </si>
 </sst>
 </file>
@@ -109,7 +103,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,18 +116,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -382,55 +364,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,194 +692,211 @@
   <dimension ref="C3:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C19" sqref="C19:N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="42" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
+    <row r="3" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="11" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="7" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="10" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="10" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="C19:N19"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="G10:H10"/>
@@ -911,23 +906,6 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:H15" xr:uid="{7956206A-2EFF-4B64-A1C0-B0E2EBA19354}">

</xml_diff>